<commit_message>
change functional component to class and add lifecycle actions
</commit_message>
<xml_diff>
--- a/zennolabchat.xlsx
+++ b/zennolabchat.xlsx
@@ -432,264 +432,258 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Vladimir</v>
+        <v>Михаил</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Зубенко</v>
       </c>
       <c r="C3" t="str">
-        <v>kagorec</v>
+        <v>maafi0znik</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>.</v>
+        <v>Gera</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Gio</v>
       </c>
       <c r="C4" t="str">
-        <v>uptget</v>
+        <v>geragioOF</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Андрей</v>
+        <v>Nova</v>
       </c>
       <c r="C5" t="str">
-        <v>ankurby</v>
+        <v>z3roonez</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Василий</v>
+        <v>Dan</v>
       </c>
       <c r="C6" t="str">
-        <v>DerTopf</v>
+        <v>Danmandrik</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Black</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Shark</v>
-      </c>
-      <c r="D7" t="str">
-        <v>79292678681</v>
+        <v>Garry</v>
+      </c>
+      <c r="C7" t="str">
+        <v>GarryTrueman</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Br1tva</v>
+        <v>Виталя</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Vitalya3639</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Вадим</v>
+        <v>Angel🔞</v>
       </c>
       <c r="C9" t="str">
-        <v>anton100800</v>
+        <v>Nikkikis</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Kayfaric</v>
+        <v>cmvvo</v>
       </c>
       <c r="C10" t="str">
-        <v>Samoregovich</v>
+        <v>cmvvo</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Рома</v>
+        <v>Saf</v>
       </c>
       <c r="B11" t="str">
-        <v>Опарин</v>
+        <v>666</v>
       </c>
       <c r="C11" t="str">
-        <v>RomaOparin</v>
+        <v>faggio666</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Руслан</v>
+        <v>My</v>
       </c>
       <c r="B12" t="str">
-        <v>Шарафутдинов</v>
+        <v>World</v>
       </c>
       <c r="C12" t="str">
-        <v>sharafutdinov_ruslan</v>
+        <v>usernameisgood</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Gogoleff</v>
+        <v>Global</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Freelance</v>
       </c>
       <c r="C13" t="str">
-        <v>Gogoleff17</v>
+        <v>Global_Freelance</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Артем</v>
+        <v>Vadler</v>
       </c>
       <c r="B14" t="str">
-        <v>Новичков</v>
+        <v>Scott</v>
       </c>
       <c r="C14" t="str">
-        <v>Favseller</v>
+        <v>PavelVadler</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Грязный Марио</v>
+        <v>Игорь</v>
       </c>
       <c r="C15" t="str">
-        <v>plsalisvern</v>
+        <v>Igor962</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Aleksandr</v>
+        <v>Ел</v>
       </c>
       <c r="B16" t="str">
-        <v>Op</v>
-      </c>
-      <c r="C16" t="str">
-        <v>aleks00p</v>
+        <v>Бол</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Дмитрий</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Сапожников</v>
+        <v>🅼🆁🎩🆅🅰️🅻</v>
       </c>
       <c r="C17" t="str">
-        <v>senorsap</v>
+        <v>ValentinKuratov</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Toxa</v>
+        <v>Игорь</v>
       </c>
       <c r="C18" t="str">
-        <v>maktoxa</v>
+        <v>eeek01</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Mark</v>
+        <v>Law Abiding</v>
       </c>
       <c r="B19" t="str">
-        <v>West</v>
+        <v>Citizen</v>
       </c>
       <c r="C19" t="str">
-        <v>markfoff</v>
+        <v>i_am_lac</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>BPH</v>
+        <v>Ivan</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Milov</v>
       </c>
       <c r="C20" t="str">
-        <v>BountyProgramHunter</v>
+        <v>ivan_milov</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>rathor</v>
-      </c>
-      <c r="B21" t="str">
-        <v>vasta</v>
+        <v>m</v>
       </c>
       <c r="C21" t="str">
-        <v>lisk22</v>
+        <v>temp_username1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Дm</v>
+        <v>networkcat</v>
       </c>
       <c r="C22" t="str">
-        <v>Gjmmml</v>
+        <v>networkcat</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Weberd</v>
+        <v>Герман</v>
       </c>
       <c r="C23" t="str">
-        <v>weberd</v>
+        <v>German_Donbass</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Olga</v>
+        <v>Aleksandr</v>
       </c>
       <c r="C24" t="str">
-        <v>olainweb</v>
+        <v>skul0n</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Forest</v>
+        <v>Bogdan</v>
       </c>
       <c r="C25" t="str">
-        <v>F_orest</v>
+        <v>BogdanUA</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Sergey</v>
+        <v>Денис</v>
       </c>
       <c r="C26" t="str">
-        <v>silverik</v>
+        <v>tashlyk</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Бро</v>
+        <v>Pass</v>
       </c>
       <c r="C27" t="str">
-        <v>Broo_m</v>
+        <v>Pass_go</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Лёвин</v>
-      </c>
-      <c r="B28" t="str">
-        <v>Владимир</v>
+        <v>Эдуард</v>
       </c>
       <c r="C28" t="str">
-        <v>Levinvladimir</v>
+        <v>Eduard_Mikhailov</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>cor</v>
+        <v>Fox SPb 🇪🇺</v>
       </c>
       <c r="C29" t="str">
-        <v>forceneo</v>
+        <v>fox_work</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Michael</v>
-      </c>
-      <c r="B30" t="str">
-        <v>Mavromatis</v>
+        <v>SEGAL</v>
       </c>
       <c r="C30" t="str">
-        <v>Mihalakis</v>
+        <v>segal1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Traffic</v>
-      </c>
-      <c r="B31" t="str">
-        <v>VooDoo</v>
+        <v>Iren</v>
       </c>
       <c r="C31" t="str">
-        <v>Traffic_VooDoo</v>
+        <v>Irennna</v>
       </c>
     </row>
   </sheetData>

</xml_diff>